<commit_message>
responsive text using ggfittext
</commit_message>
<xml_diff>
--- a/manuscript/data/zhf_extracted.xlsx
+++ b/manuscript/data/zhf_extracted.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yangke17\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roseannaconway/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20240" windowHeight="14360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="87">
   <si>
     <t>n</t>
   </si>
@@ -276,12 +282,27 @@
   </si>
   <si>
     <t>Funding/equipment/conflict comment</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>tertiary</t>
+  </si>
+  <si>
+    <t>quarternary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -328,16 +349,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -696,135 +717,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D32" sqref="D32"/>
+      <selection pane="topRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="33.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="36.140625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="3"/>
-    <col min="18" max="18" width="39" customWidth="1"/>
+    <col min="1" max="2" width="28.5" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="33.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="36.1640625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="10" customWidth="1"/>
+    <col min="15" max="15" width="20.33203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.1640625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" style="3"/>
+    <col min="19" max="19" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="2">
-        <v>103</v>
+      <c r="B2" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C2" s="2">
         <v>103</v>
       </c>
       <c r="D2" s="2">
+        <v>103</v>
+      </c>
+      <c r="E2" s="2">
         <v>35717</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>-0.23</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>-1.05</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>0.59</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O2" s="3" t="s">
         <v>25</v>
       </c>
@@ -834,56 +858,57 @@
       <c r="Q2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="14" t="s">
-        <v>6</v>
+      <c r="R2" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="S2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="2">
-        <v>103</v>
-      </c>
+      <c r="B3" s="4"/>
       <c r="C3" s="2">
         <v>103</v>
       </c>
       <c r="D3" s="2">
+        <v>103</v>
+      </c>
+      <c r="E3" s="2">
         <v>13929</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>-0.08</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>-0.96</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>0.8</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O3" s="3" t="s">
         <v>25</v>
       </c>
@@ -893,55 +918,56 @@
       <c r="Q3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="14" t="s">
-        <v>6</v>
+      <c r="R3" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="S3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="2">
-        <v>103</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="2">
         <v>103</v>
       </c>
       <c r="D4" s="2">
+        <v>103</v>
+      </c>
+      <c r="E4" s="2">
         <v>21788</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>-0.32</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>-1.07</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>0.43</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>4</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>25</v>
+      <c r="N4" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>25</v>
@@ -952,172 +978,177 @@
       <c r="Q4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="14" t="s">
-        <v>6</v>
+      <c r="R4" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="S4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T4" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="2">
-        <v>83</v>
-      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="2">
         <v>83</v>
       </c>
       <c r="D5" s="2">
+        <v>83</v>
+      </c>
+      <c r="E5" s="2">
         <v>249</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>-0.35</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>-0.91839999999999999</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>0.21840000000000001</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>3</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>26</v>
+      <c r="P5" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="S5" s="3" t="s">
+      <c r="R5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="T5" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="2">
-        <v>83</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="2">
         <v>83</v>
       </c>
       <c r="D6" s="2">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2">
         <v>249</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>-0.34160000000000001</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>0.48159999999999997</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="N6" s="10" t="s">
         <v>3</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>26</v>
+      <c r="P6" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R6" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="S6" s="3" t="s">
+      <c r="R6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="2">
-        <v>15</v>
+      <c r="B7" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C7" s="2">
         <v>15</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3">
+      <c r="D7" s="2">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3">
         <v>0.08</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>-0.25</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>0.4</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="M7" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="N7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O7" s="3" t="s">
         <v>25</v>
       </c>
@@ -1127,54 +1158,57 @@
       <c r="Q7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R7" s="14" t="s">
-        <v>6</v>
+      <c r="R7" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="S7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="2">
-        <v>15</v>
+      <c r="B8" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="C8" s="2">
         <v>15</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3">
+      <c r="D8" s="2">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3">
         <v>-0.05</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>-0.56000000000000005</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>0.47</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="M8" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="N8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O8" s="3" t="s">
         <v>25</v>
       </c>
@@ -1184,54 +1218,55 @@
       <c r="Q8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="14" t="s">
-        <v>6</v>
+      <c r="R8" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="S8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T8" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="2">
-        <v>15</v>
-      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="2">
         <v>15</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3">
+      <c r="D9" s="2">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3">
         <v>-0.12</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>-0.94</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>0.71</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="M9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="N9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1241,56 +1276,59 @@
       <c r="Q9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R9" s="14" t="s">
-        <v>6</v>
+      <c r="R9" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="S9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T9" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="2">
-        <v>22</v>
+      <c r="B10" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C10" s="2">
         <v>22</v>
       </c>
       <c r="D10" s="2">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2">
         <v>1708</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>-0.1</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>-0.5</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>0.3</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="M10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="N10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O10" s="3" t="s">
         <v>25</v>
       </c>
@@ -1300,54 +1338,57 @@
       <c r="Q10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="S10" s="3" t="s">
+      <c r="R10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T10" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2">
+      <c r="B11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <v>22</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>72</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>0.5</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>-1.2</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="M11" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="M11" s="10" t="s">
+      <c r="N11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O11" s="3" t="s">
         <v>25</v>
       </c>
@@ -1357,56 +1398,59 @@
       <c r="Q11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="S11" s="3" t="s">
+      <c r="R11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T11" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="2">
-        <v>49</v>
+      <c r="B12" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C12" s="2">
         <v>49</v>
       </c>
       <c r="D12" s="2">
+        <v>49</v>
+      </c>
+      <c r="E12" s="2">
         <v>3245</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>0.1</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>-0.4</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>0.6</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="M12" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="N12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N12" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1416,54 +1460,57 @@
       <c r="Q12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="S12" s="3" t="s">
+      <c r="R12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T12" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2">
+      <c r="B13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <v>49</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>101</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="3">
         <v>0.6</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>-1.2</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>2.4</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="M13" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="N13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O13" s="3" t="s">
         <v>25</v>
       </c>
@@ -1473,226 +1520,236 @@
       <c r="Q13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="S13" s="3" t="s">
+      <c r="R13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T13" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="2">
-        <v>29</v>
-      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="2">
         <v>29</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3">
+      <c r="D14" s="2">
+        <v>29</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3">
         <v>0.11</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>-0.54</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>0.75</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="M14" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="N14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="O14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="P14" s="3" t="s">
         <v>25</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R14" s="14" t="s">
-        <v>6</v>
+      <c r="R14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="S14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T14" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="2">
-        <v>29</v>
+      <c r="B15" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C15" s="2">
         <v>29</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3">
+      <c r="D15" s="2">
+        <v>29</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>-0.81</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>0.52</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="M15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M15" s="10" t="s">
+      <c r="N15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="O15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O15" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="P15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="S15" s="14" t="s">
+      <c r="R15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="T15" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="2">
-        <v>54</v>
+      <c r="B16" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C16" s="2">
         <v>54</v>
       </c>
       <c r="D16" s="2">
+        <v>54</v>
+      </c>
+      <c r="E16" s="2">
         <v>1664</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
         <v>-0.39</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>0.66</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="M16" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M16" s="10" t="s">
+      <c r="N16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="O16" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="P16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="Q16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R16" s="14" t="s">
+      <c r="S16" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="2">
-        <v>7</v>
+      <c r="B17" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C17" s="2">
         <v>7</v>
       </c>
       <c r="D17" s="2">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2">
         <v>1850</v>
       </c>
-      <c r="E17" s="3">
+      <c r="F17" s="3">
         <v>0</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>-0.36</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>0.36</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="M17" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M17" s="10" t="s">
+      <c r="N17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="N17" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O17" s="3" t="s">
         <v>25</v>
       </c>
@@ -1702,56 +1759,59 @@
       <c r="Q17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R17" s="14" t="s">
-        <v>6</v>
+      <c r="R17" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="S17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T17" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="2">
-        <v>52</v>
+      <c r="B18" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="C18" s="2">
         <v>52</v>
       </c>
       <c r="D18" s="2">
+        <v>52</v>
+      </c>
+      <c r="E18" s="2">
         <v>61298</v>
       </c>
-      <c r="E18" s="3">
+      <c r="F18" s="3">
         <v>-0.19</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>-0.72</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>0.34</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="M18" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M18" s="10" t="s">
+      <c r="N18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="N18" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1761,55 +1821,58 @@
       <c r="Q18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R18" s="14" t="s">
-        <v>6</v>
+      <c r="R18" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="S18" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T18" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="2">
-        <v>26</v>
+      <c r="B19" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C19" s="2">
         <v>26</v>
       </c>
       <c r="D19" s="2">
+        <v>26</v>
+      </c>
+      <c r="E19" s="2">
         <v>53495</v>
       </c>
-      <c r="E19" s="3">
+      <c r="F19" s="3">
         <v>0.82</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="3">
         <v>0.31</v>
       </c>
-      <c r="G19" s="3">
+      <c r="H19" s="3">
         <v>1.33</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="M19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M19" s="10" t="s">
+      <c r="N19" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="O19" s="6" t="s">
         <v>27</v>
@@ -1820,112 +1883,118 @@
       <c r="Q19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R19" s="15" t="s">
+      <c r="R19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="S19" s="15"/>
-    </row>
-    <row r="20" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T19" s="15"/>
+    </row>
+    <row r="20" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="2">
-        <v>29</v>
+      <c r="B20" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C20" s="2">
         <v>29</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="2">
+        <v>29</v>
+      </c>
+      <c r="E20" s="8">
         <v>2511</v>
       </c>
-      <c r="E20" s="3">
+      <c r="F20" s="3">
         <v>0.02</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>-0.5</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>0.5</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="M20" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="N20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O20" s="6" t="s">
+      <c r="O20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="P20" s="6" t="s">
+      <c r="Q20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Q20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R20" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="S20" s="15" t="s">
+      <c r="R20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S20" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T20" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="2">
-        <v>20</v>
+      <c r="B21" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C21" s="2">
         <v>20</v>
       </c>
       <c r="D21" s="2">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
         <v>16407</v>
       </c>
-      <c r="E21" s="3">
+      <c r="F21" s="3">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>-1.1599999999999999</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>0.6</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L21" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="M21" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M21" s="10" t="s">
+      <c r="N21" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="O21" s="6" t="s">
         <v>27</v>
@@ -1936,108 +2005,114 @@
       <c r="Q21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R21" s="15" t="s">
+      <c r="R21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S21" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="2">
-        <v>66</v>
+      <c r="B22" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C22" s="2">
         <v>66</v>
       </c>
       <c r="D22" s="2">
+        <v>66</v>
+      </c>
+      <c r="E22" s="2">
         <v>401</v>
       </c>
-      <c r="E22" s="3">
+      <c r="F22" s="3">
         <v>-0.27</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="3">
         <v>-0.61</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L22" s="10" t="s">
+      <c r="M22" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M22" s="10" t="s">
+      <c r="N22" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="O22" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Q22" s="3" t="s">
+      <c r="Q22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R22" s="15" t="s">
+      <c r="S22" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="2">
-        <v>9</v>
+      <c r="B23" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C23" s="2">
         <v>9</v>
       </c>
       <c r="D23" s="2">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2">
         <v>180</v>
       </c>
-      <c r="E23" s="3">
+      <c r="F23" s="3">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="F23" s="3">
+      <c r="G23" s="3">
         <v>-0.54</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="3">
         <v>0.4</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L23" s="10" t="s">
+      <c r="M23" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M23" s="10" t="s">
+      <c r="N23" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>26</v>
@@ -2045,55 +2120,58 @@
       <c r="P23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q23" s="6" t="s">
+      <c r="Q23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R23" s="15" t="s">
+      <c r="S23" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="2">
-        <v>29</v>
+      <c r="B24" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="C24" s="2">
         <v>29</v>
       </c>
       <c r="D24" s="2">
+        <v>29</v>
+      </c>
+      <c r="E24" s="2">
         <v>580</v>
       </c>
-      <c r="E24" s="3">
+      <c r="F24" s="3">
         <v>-0.24</v>
       </c>
-      <c r="F24" s="3">
+      <c r="G24" s="3">
         <v>-0.81</v>
       </c>
-      <c r="G24" s="3">
+      <c r="H24" s="3">
         <v>0.33</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L24" s="10" t="s">
+      <c r="M24" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M24" s="10" t="s">
+      <c r="N24" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>26</v>
@@ -2101,56 +2179,59 @@
       <c r="P24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q24" s="6" t="s">
+      <c r="Q24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R24" s="15" t="s">
+      <c r="S24" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="2">
-        <v>10</v>
+      <c r="B25" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C25" s="2">
         <v>10</v>
       </c>
       <c r="D25" s="2">
+        <v>10</v>
+      </c>
+      <c r="E25" s="2">
         <v>303</v>
       </c>
-      <c r="E25" s="3">
+      <c r="F25" s="3">
         <v>0.01</v>
       </c>
-      <c r="F25" s="3">
+      <c r="G25" s="3">
         <v>-0.47</v>
       </c>
-      <c r="G25" s="3">
+      <c r="H25" s="3">
         <v>0.49</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J25" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L25" s="10" t="s">
+      <c r="M25" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M25" s="12" t="s">
+      <c r="N25" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N25" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="O25" s="3" t="s">
         <v>25</v>
       </c>
@@ -2160,181 +2241,189 @@
       <c r="Q25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R25" s="15" t="s">
+      <c r="R25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S25" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="2">
-        <v>170</v>
-      </c>
+      <c r="B26" s="4"/>
       <c r="C26" s="2">
         <v>170</v>
       </c>
       <c r="D26" s="2">
+        <v>170</v>
+      </c>
+      <c r="E26" s="2">
         <v>109570</v>
       </c>
-      <c r="E26" s="3">
+      <c r="F26" s="3">
         <v>-0.11</v>
       </c>
-      <c r="F26" s="3">
+      <c r="G26" s="3">
         <v>-0.75</v>
       </c>
-      <c r="G26" s="3">
+      <c r="H26" s="3">
         <v>0.53</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J26" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L26" s="10" t="s">
+      <c r="M26" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M26" s="12" t="s">
+      <c r="N26" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N26" s="6" t="s">
+      <c r="O26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O26" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="P26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R26" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="S26" s="14" t="s">
+      <c r="R26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S26" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="T26" s="14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="2">
-        <v>24</v>
-      </c>
+      <c r="B27" s="4"/>
       <c r="C27" s="2">
         <v>24</v>
       </c>
       <c r="D27" s="2">
+        <v>24</v>
+      </c>
+      <c r="E27" s="2">
         <v>22482</v>
       </c>
-      <c r="E27" s="3">
+      <c r="F27" s="3">
         <v>-0.06</v>
       </c>
-      <c r="F27" s="3">
+      <c r="G27" s="3">
         <v>-0.64</v>
       </c>
-      <c r="G27" s="3">
+      <c r="H27" s="3">
         <v>0.52</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="I27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J27" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="K27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L27" s="10" t="s">
+      <c r="M27" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M27" s="12" t="s">
+      <c r="N27" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N27" s="6" t="s">
+      <c r="O27" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O27" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="P27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="S27" s="14" t="s">
+      <c r="R27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="T27" s="14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="2">
-        <v>41</v>
+      <c r="B28" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C28" s="2">
         <v>41</v>
       </c>
       <c r="D28" s="2">
+        <v>41</v>
+      </c>
+      <c r="E28" s="2">
         <v>289</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>0.21</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>-2.27</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>2.71</v>
       </c>
-      <c r="H28" t="s">
-        <v>6</v>
-      </c>
       <c r="I28" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" t="s">
         <v>2</v>
       </c>
-      <c r="J28" t="s">
-        <v>6</v>
-      </c>
       <c r="K28" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" t="s">
         <v>16</v>
       </c>
-      <c r="L28" s="10" t="s">
+      <c r="M28" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M28" s="12" t="s">
+      <c r="N28" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N28" s="6" t="s">
+      <c r="O28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O28" s="3" t="s">
+      <c r="P28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P28" s="3" t="s">
+      <c r="Q28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R28" s="15" t="s">
+      <c r="R28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S28" s="15" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started R1 for jcmc
</commit_message>
<xml_diff>
--- a/manuscript/data/zhf_extracted.xlsx
+++ b/manuscript/data/zhf_extracted.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronconway/zhf-review/manuscript/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64096DAC-AB95-2941-9B41-50B4FA827912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D54B021-7A7F-F242-AD23-4A7F1612B8F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="640" windowWidth="31740" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="88">
   <si>
     <t>n</t>
   </si>
@@ -303,18 +303,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>Sastre, 2019</t>
-  </si>
-  <si>
-    <t>Harioka, 2000</t>
-  </si>
-  <si>
-    <t>Abdominal and thoracic surgery</t>
-  </si>
-  <si>
-    <t>Drägerwerk AG &amp; Co (Germany) provided the Tcore™ thermometer used for the study. </t>
   </si>
 </sst>
 </file>
@@ -739,7 +727,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H30" sqref="H30"/>
+      <selection pane="topRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2499,179 +2487,33 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="2">
-        <v>40</v>
-      </c>
-      <c r="D30" s="2">
-        <v>40</v>
-      </c>
-      <c r="E30" s="2">
-        <v>640</v>
-      </c>
-      <c r="F30" s="2">
-        <v>-0.2</v>
-      </c>
-      <c r="G30" s="2">
-        <v>-1.4</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="I30" t="s">
-        <v>6</v>
-      </c>
-      <c r="J30" t="s">
-        <v>2</v>
-      </c>
-      <c r="K30" t="s">
-        <v>6</v>
-      </c>
-      <c r="L30" t="s">
-        <v>55</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="N30" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="O30" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P30" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q30" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="R30" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="S30" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="T30" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="2">
-        <v>40</v>
-      </c>
-      <c r="E31" s="2">
-        <v>960</v>
-      </c>
-      <c r="F31">
-        <v>-0.2</v>
-      </c>
-      <c r="G31" s="2">
-        <v>-1.29</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0.89</v>
-      </c>
-      <c r="I31" t="s">
-        <v>6</v>
-      </c>
-      <c r="J31" t="s">
-        <v>8</v>
-      </c>
-      <c r="K31" t="s">
-        <v>6</v>
-      </c>
-      <c r="L31" t="s">
-        <v>55</v>
-      </c>
-      <c r="M31" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="N31" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P31" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q31" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="R31" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="S31" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="T31" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="2">
-        <v>41</v>
-      </c>
-      <c r="D32" s="2">
-        <v>41</v>
-      </c>
-      <c r="E32" s="2">
-        <v>451</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>-0.6</v>
-      </c>
-      <c r="H32">
-        <v>0.6</v>
-      </c>
-      <c r="I32" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" t="s">
-        <v>2</v>
-      </c>
-      <c r="K32" t="s">
-        <v>6</v>
-      </c>
-      <c r="L32" t="s">
-        <v>90</v>
-      </c>
-      <c r="M32" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="N32" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P32" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q32" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="R32" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="S32" s="15" t="s">
-        <v>12</v>
-      </c>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="14"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="14"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O32" s="6"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>